<commit_message>
Adding components to schematic
</commit_message>
<xml_diff>
--- a/Documentation/BOM.xlsx
+++ b/Documentation/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">Part</t>
   </si>
@@ -61,10 +61,10 @@
     <t xml:space="preserve">MOSFET</t>
   </si>
   <si>
-    <t xml:space="preserve">IRFS7437TRL7PP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/infineon-technologies/IRFS7437TRL7PP/3712564</t>
+    <t xml:space="preserve">TPH2R608NH,L1Q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/toshiba-semiconductor-and-storage/TPH2R608NH-L1Q/5456312</t>
   </si>
   <si>
     <t xml:space="preserve">Current Sense</t>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t xml:space="preserve">Micro-JST 6PIN 2mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5v to 3.3v buck converter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LM3671</t>
   </si>
 </sst>
 </file>
@@ -141,6 +147,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -218,10 +225,10 @@
   <dimension ref="C4:H26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.62"/>
@@ -303,14 +310,14 @@
         <v>13</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>2.655</v>
+        <v>1.64</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>10</v>
       </c>
       <c r="G8" s="0" t="n">
         <f aca="false">E8*F8</f>
-        <v>26.55</v>
+        <v>16.4</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>14</v>
@@ -392,6 +399,12 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>27</v>
+      </c>
       <c r="G13" s="0" t="n">
         <f aca="false">E13*F13</f>
         <v>0</v>
@@ -479,7 +492,7 @@
   <hyperlinks>
     <hyperlink ref="H5" r:id="rId1" display="https://surpasshobbyusa.net/rocket-v5r-spec-10-5t-sensored-brushless-motor-silver-black/v5r-10-5/"/>
     <hyperlink ref="H6" r:id="rId2" display="https://genstattu.com/gens-ace-5000mah-11-1v-60c-3s1p-short-size-lipo-battery-pack-with-xt60-plug/"/>
-    <hyperlink ref="H8" r:id="rId3" display="https://www.digikey.com/en/products/detail/infineon-technologies/IRFS7437TRL7PP/3712564"/>
+    <hyperlink ref="H8" r:id="rId3" display="https://www.digikey.com/en/products/detail/toshiba-semiconductor-and-storage/TPH2R608NH-L1Q/5456312"/>
     <hyperlink ref="H9" r:id="rId4" display="https://www.digikey.com/en/products/detail/analog-devices-inc/AD8418AWBRZ-RL/4901146"/>
     <hyperlink ref="H10" r:id="rId5" display="https://www.digikey.com/en/products/detail/nxp-usa-inc/TJA1051AT-0Z/10815355"/>
     <hyperlink ref="H11" r:id="rId6" display="https://www.mouser.com/ProductDetail/Texas-Instruments/UCC27211AQDDARQ1?qs=n%252BTO0c4TDSYQNOcAHEGCfA%3D%3D"/>

</xml_diff>